<commit_message>
Excel export/import + Almanac page
</commit_message>
<xml_diff>
--- a/src/assets/import-template/import_template.xlsx
+++ b/src/assets/import-template/import_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61D7B270-EBD9-4719-AA52-0D93EF74A3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{137B60D9-7A9B-4DBA-9DAC-B3A9E4D735C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Champions" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Abilities" sheetId="3" r:id="rId3"/>
     <sheet name="Monsters" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>HP</t>
   </si>
   <si>
-    <t>Base Damage</t>
+    <t>Damage</t>
   </si>
   <si>
     <t>Price</t>
@@ -56,7 +56,7 @@
     <t>Bonus Damage</t>
   </si>
   <si>
-    <t>Bonus Hp</t>
+    <t>Bonus HP</t>
   </si>
   <si>
     <t>Type</t>
@@ -65,9 +65,6 @@
     <t>Healing</t>
   </si>
   <si>
-    <t>Damage</t>
-  </si>
-  <si>
     <t>Mana Cost</t>
   </si>
   <si>
@@ -83,34 +80,25 @@
     <t>Money Reward</t>
   </si>
   <si>
-    <t>Exp Reward</t>
+    <t>EXP Reward</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,17 +124,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -455,25 +441,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25">
+    <row r="1" spans="1:7" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,24 +477,6 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="21">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="21">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -520,44 +484,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79532E6F-44E7-42D6-9243-34AB67544740}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970A3C47-AE7E-4462-9142-C652B5C4E20F}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -567,45 +531,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023806F6-14DE-46E6-BEB9-366F19AD34BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C817A64A-8469-42A6-9800-32819C73F588}">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -614,48 +578,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0DA5883-AC52-4C7E-8D22-587F652CCC7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866EEDA1-6F41-4D9D-8936-84E6830C7F71}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>